<commit_message>
Code made to manipulate data to handle seasons properly. Excel file created to store outputs. App code modified to point to new datasource
</commit_message>
<xml_diff>
--- a/filtered_table_data.xlsx
+++ b/filtered_table_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Jack\Desktop\stardew-fishing-helper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF0ADFC-1872-4CB1-94A0-58CC8B059E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D351BA-BC12-4BBA-8C85-9E461C529376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$C$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$C$48</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,20 +36,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="130">
   <si>
     <t>Pufferfish</t>
   </si>
   <si>
-    <t>Ocean, Ginger Island oceans</t>
-  </si>
-  <si>
     <t>12pm – 4pm</t>
   </si>
   <si>
-    <t>Summer(All Seasons on Ginger Island)</t>
-  </si>
-  <si>
     <t>Sun</t>
   </si>
   <si>
@@ -74,9 +68,6 @@
     <t>6am – 7pm</t>
   </si>
   <si>
-    <t>Summer Winter(All Seasons on Ginger Island)</t>
-  </si>
-  <si>
     <t>Sardine</t>
   </si>
   <si>
@@ -200,9 +191,6 @@
     <t>Super Cucumber</t>
   </si>
   <si>
-    <t>Summer Fall(All Seasons on Ginger Island)</t>
-  </si>
-  <si>
     <t>Ghostfish</t>
   </si>
   <si>
@@ -236,18 +224,12 @@
     <t>Flounder</t>
   </si>
   <si>
-    <t>Spring Summer(All Seasons on Ginger Island)</t>
-  </si>
-  <si>
     <t>Midnight Carp</t>
   </si>
   <si>
     <t>10pm – 2am</t>
   </si>
   <si>
-    <t>Fall Winter(All Seasons on Ginger Island)</t>
-  </si>
-  <si>
     <t>Sturgeon</t>
   </si>
   <si>
@@ -263,9 +245,6 @@
     <t>Tilapia</t>
   </si>
   <si>
-    <t>Ocean, Ginger Island rivers</t>
-  </si>
-  <si>
     <t>6am – 2pm</t>
   </si>
   <si>
@@ -323,24 +302,6 @@
     <t>Mutant Bug Lair</t>
   </si>
   <si>
-    <t>Stingray</t>
-  </si>
-  <si>
-    <t>Pirate Cove (Ginger Island)</t>
-  </si>
-  <si>
-    <t>Lionfish</t>
-  </si>
-  <si>
-    <t>Ginger Island Ocean</t>
-  </si>
-  <si>
-    <t>Blue Discus</t>
-  </si>
-  <si>
-    <t>Ginger Island Pond and Rivers</t>
-  </si>
-  <si>
     <t>Goby</t>
   </si>
   <si>
@@ -437,24 +398,15 @@
     <t>The Mountain Lake, Secret Woods Pond, The Sewers</t>
   </si>
   <si>
-    <t>River (Town+Forest), Secret Woods Pond, Witch's Swamp</t>
-  </si>
-  <si>
     <t>River (Town+Forest), Forest Pond</t>
   </si>
   <si>
     <t>The Mines 20F &amp; 60F, Ghost drops</t>
   </si>
   <si>
-    <t>The Mines 100F, Volcano Caldera</t>
-  </si>
-  <si>
     <t>The Desert (Requires fishing level 4)</t>
   </si>
   <si>
-    <t>Mountain Lake, Cindersap Forest pond, Ginger Island pond and river</t>
-  </si>
-  <si>
     <t>Cindersap Forest River, Mountain Lake</t>
   </si>
   <si>
@@ -462,6 +414,18 @@
   </si>
   <si>
     <t>Secret Woods Pond, Forest Farm</t>
+  </si>
+  <si>
+    <t>River (Town+Forest), Secret Woods Pond</t>
+  </si>
+  <si>
+    <t>The Mines 100F</t>
+  </si>
+  <si>
+    <t>Mountain Lake, Cindersap Forest pond</t>
+  </si>
+  <si>
+    <t>Summer Fall</t>
   </si>
 </sst>
 </file>
@@ -517,8 +481,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{612B687C-F04F-48CC-B05F-D4A50728FC2C}" name="Table1" displayName="Table1" ref="A1:I49" totalsRowShown="0">
-  <autoFilter ref="A1:I49" xr:uid="{612B687C-F04F-48CC-B05F-D4A50728FC2C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{612B687C-F04F-48CC-B05F-D4A50728FC2C}" name="Table1" displayName="Table1" ref="A1:I46" totalsRowShown="0">
+  <autoFilter ref="A1:I46" xr:uid="{612B687C-F04F-48CC-B05F-D4A50728FC2C}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{651714FE-BF8A-4E94-A5D7-C623508A50E6}" name="Fish"/>
     <tableColumn id="2" xr3:uid="{A8B896FD-D6AB-4C12-BD77-C2BB95B0402E}" name="Location"/>
@@ -823,10 +787,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:XFD53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,7 +798,7 @@
     <col min="1" max="1" width="19.28515625" customWidth="1"/>
     <col min="2" max="2" width="70.140625" customWidth="1"/>
     <col min="3" max="3" width="29.140625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="50.5703125" customWidth="1"/>
+    <col min="4" max="4" width="73.42578125" customWidth="1"/>
     <col min="5" max="5" width="44.5703125" customWidth="1"/>
     <col min="6" max="6" width="12.140625" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="30.140625" hidden="1" customWidth="1"/>
@@ -844,31 +808,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="B1" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="C1" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="D1" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="E1" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="F1" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="G1" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="H1" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="I1" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -876,22 +840,22 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
       <c r="F2" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="G2" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="H2" t="str">
         <f>IF(F2=$F$3,$F$4,F2)</f>
@@ -904,53 +868,53 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H49" si="0">IF(F3=$F$3,$F$4,F3)</f>
+        <f t="shared" ref="H3:H46" si="0">IF(F3=$F$3,$F$4,F3)</f>
         <v xml:space="preserve">6am </v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I49" si="1">IF(G3=$G$3,$G$11,G3)</f>
+        <f t="shared" ref="I3:I46" si="1">IF(G3=$G$3,$G$11,G3)</f>
         <v xml:space="preserve"> 2am</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="G4" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
@@ -963,25 +927,25 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="G5" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
@@ -994,25 +958,25 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="G6" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
@@ -1025,25 +989,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="G7" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
@@ -1056,22 +1020,22 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
@@ -1084,25 +1048,25 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="G9" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
@@ -1115,25 +1079,25 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F10" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="G10" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
@@ -1146,25 +1110,25 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
         <v>26</v>
       </c>
-      <c r="B11" t="s">
-        <v>131</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" t="s">
-        <v>29</v>
-      </c>
       <c r="F11" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="G11" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
@@ -1177,22 +1141,22 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
@@ -1205,22 +1169,22 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
@@ -1233,25 +1197,25 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F14" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="G14" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
@@ -1264,22 +1228,22 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
@@ -1292,25 +1256,25 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F16" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="G16" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
@@ -1323,25 +1287,25 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E17" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F17" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="G17" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
@@ -1354,22 +1318,22 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E18" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F18" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
@@ -1382,25 +1346,25 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" t="s">
         <v>6</v>
       </c>
-      <c r="C19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" t="s">
-        <v>8</v>
-      </c>
       <c r="E19" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F19" t="s">
-        <v>117</v>
+        <v>104</v>
       </c>
       <c r="G19" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
@@ -1413,25 +1377,25 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="E20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F20" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="G20" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
@@ -1444,25 +1408,25 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F21" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="G21" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
@@ -1475,25 +1439,25 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F22" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="G22" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
@@ -1506,25 +1470,25 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E23" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F23" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="G23" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
@@ -1537,25 +1501,25 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B24" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="E24" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F24" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="G24" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
@@ -1568,22 +1532,22 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F25" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
@@ -1596,22 +1560,22 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E26" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F26" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
@@ -1624,22 +1588,22 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E27" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F27" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
@@ -1652,22 +1616,22 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B28" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C28" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E28" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F28" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
@@ -1680,25 +1644,25 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C29" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D29" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E29" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F29" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="G29" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="0"/>
@@ -1711,25 +1675,25 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B30" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="C30" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D30" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E30" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F30" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="G30" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="0"/>
@@ -1742,25 +1706,25 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B31" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D31" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="E31" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F31" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="G31" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="0"/>
@@ -1773,25 +1737,25 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B32" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="C32" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D32" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="E32" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F32" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="G32" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="0"/>
@@ -1804,25 +1768,25 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C33" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D33" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E33" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F33" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="G33" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="0"/>
@@ -1835,25 +1799,25 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B34" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C34" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D34" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E34" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F34" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="G34" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="0"/>
@@ -1866,22 +1830,22 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B35" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C35" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E35" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F35" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="0"/>
@@ -1894,25 +1858,25 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B36" t="s">
-        <v>75</v>
+        <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D36" t="s">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="E36" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F36" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="G36" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="0"/>
@@ -1925,22 +1889,22 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B37" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="C37" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E37" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F37" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="0"/>
@@ -1953,25 +1917,25 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B38" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C38" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D38" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E38" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F38" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="G38" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="0"/>
@@ -1984,25 +1948,25 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D39" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E39" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F39" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="G39" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="H39" t="str">
         <f>IF(F39=$F$3,$F$4,F39)</f>
@@ -2015,25 +1979,25 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B40" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D40" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E40" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F40" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="G40" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="H40" t="str">
         <f t="shared" si="0"/>
@@ -2046,22 +2010,22 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B41" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="C41" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D41" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E41" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F41" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="H41" t="str">
         <f t="shared" si="0"/>
@@ -2074,25 +2038,25 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D42" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E42" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F42" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="G42" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="H42" t="str">
         <f t="shared" si="0"/>
@@ -2105,22 +2069,22 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B43" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="C43" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D43" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E43" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F43" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H43" t="str">
         <f t="shared" si="0"/>
@@ -2133,22 +2097,22 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B44" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C44" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D44" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E44" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F44" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" si="0"/>
@@ -2161,22 +2125,22 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B45" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C45" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D45" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E45" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F45" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H45" t="str">
         <f t="shared" si="0"/>
@@ -2189,112 +2153,28 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="B46" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C46" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D46" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E46" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F46" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H46" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve">6am </v>
       </c>
       <c r="I46" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> 2am</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>97</v>
-      </c>
-      <c r="B47" t="s">
-        <v>98</v>
-      </c>
-      <c r="C47" t="s">
-        <v>7</v>
-      </c>
-      <c r="D47" t="s">
-        <v>18</v>
-      </c>
-      <c r="E47" t="s">
-        <v>9</v>
-      </c>
-      <c r="F47" t="s">
-        <v>7</v>
-      </c>
-      <c r="H47" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">6am </v>
-      </c>
-      <c r="I47" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> 2am</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>99</v>
-      </c>
-      <c r="B48" t="s">
-        <v>100</v>
-      </c>
-      <c r="C48" t="s">
-        <v>7</v>
-      </c>
-      <c r="D48" t="s">
-        <v>18</v>
-      </c>
-      <c r="E48" t="s">
-        <v>9</v>
-      </c>
-      <c r="F48" t="s">
-        <v>7</v>
-      </c>
-      <c r="H48" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">6am </v>
-      </c>
-      <c r="I48" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> 2am</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>101</v>
-      </c>
-      <c r="B49" t="s">
-        <v>102</v>
-      </c>
-      <c r="C49" t="s">
-        <v>7</v>
-      </c>
-      <c r="D49" t="s">
-        <v>18</v>
-      </c>
-      <c r="E49" t="s">
-        <v>9</v>
-      </c>
-      <c r="F49" t="s">
-        <v>7</v>
-      </c>
-      <c r="H49" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">6am </v>
-      </c>
-      <c r="I49" t="str">
         <f t="shared" si="1"/>
         <v xml:space="preserve"> 2am</v>
       </c>

</xml_diff>